<commit_message>
Add majority of scripts and output
</commit_message>
<xml_diff>
--- a/data/MHH/patient_information_complete.xlsx
+++ b/data/MHH/patient_information_complete.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijnzoodsma/Documents/PhD/corona/data/MHH cohort/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijnzoodsma/Documents/PhD/corona/Postcovid-targeted-proteomics/data/MHH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A562352-F671-AA47-A46F-D18BE71672DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84D5447-1A52-1642-9E1F-4FFC50285E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="304">
   <si>
     <t>SampleID</t>
   </si>
@@ -913,9 +913,6 @@
   </si>
   <si>
     <t>antibody.S1</t>
-  </si>
-  <si>
-    <t>n.d.</t>
   </si>
   <si>
     <t/>
@@ -1411,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="E221" sqref="E221"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64:H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1457,25 +1454,25 @@
         <v>295</v>
       </c>
       <c r="I1" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>300</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -4203,12 +4200,8 @@
       <c r="F64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G64" s="30" t="s">
-        <v>296</v>
-      </c>
-      <c r="H64" s="30" t="s">
-        <v>296</v>
-      </c>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
       <c r="I64" s="17">
         <v>31.430555555555554</v>
       </c>
@@ -6014,7 +6007,7 @@
         <v>37.513888888888886</v>
       </c>
       <c r="J103" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K103" s="19"/>
       <c r="L103" s="25">
@@ -9392,7 +9385,7 @@
         <v>28.388888888888889</v>
       </c>
       <c r="J177" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K177" s="19">
         <v>2</v>

</xml_diff>